<commit_message>
Testing balance calculations with dates.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="I11:P27"/>
+  <dimension ref="I11:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +439,10 @@
         <f>J13+0.1</f>
         <v>10.1</v>
       </c>
+      <c r="L13">
+        <f>IF(K13 &lt;&gt; "",K13,J13)</f>
+        <v>10.1</v>
+      </c>
       <c r="N13">
         <v>10</v>
       </c>
@@ -446,20 +450,32 @@
         <f>N13+0.2</f>
         <v>10.199999999999999</v>
       </c>
+      <c r="P13">
+        <f>IF(O13 &lt;&gt; "",O13,N13)</f>
+        <v>10.199999999999999</v>
+      </c>
     </row>
     <row r="14" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J14">
         <v>10.01</v>
       </c>
       <c r="K14">
-        <f t="shared" ref="K14:K18" si="0">J14+0.1</f>
+        <f t="shared" ref="K14:K17" si="0">J14+0.1</f>
+        <v>10.11</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L20" si="1">IF(K14 &lt;&gt; "",K14,J14)</f>
         <v>10.11</v>
       </c>
       <c r="N14">
         <v>10.01</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O18" si="1">N14+0.2</f>
+        <f t="shared" ref="O14:O17" si="2">N14+0.2</f>
+        <v>10.209999999999999</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:P20" si="3">IF(O14 &lt;&gt; "",O14,N14)</f>
         <v>10.209999999999999</v>
       </c>
     </row>
@@ -471,27 +487,39 @@
         <f t="shared" si="0"/>
         <v>10.119999999999999</v>
       </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>10.119999999999999</v>
+      </c>
       <c r="N15">
         <v>10.02</v>
       </c>
       <c r="O15">
+        <f t="shared" si="2"/>
+        <v>10.219999999999999</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>10.219999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="1"/>
-        <v>10.219999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J16">
-        <v>10.029999999999999</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>10.129999999999999</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="N16">
         <v>10.029999999999999</v>
       </c>
       <c r="O16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>10.229999999999999</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="3"/>
         <v>10.229999999999999</v>
       </c>
     </row>
@@ -503,11 +531,19 @@
         <f t="shared" si="0"/>
         <v>10.139999999999999</v>
       </c>
+      <c r="L17">
+        <f t="shared" si="1"/>
+        <v>10.139999999999999</v>
+      </c>
       <c r="N17">
         <v>10.039999999999999</v>
       </c>
       <c r="O17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
+        <v>10.239999999999998</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="3"/>
         <v>10.239999999999998</v>
       </c>
     </row>
@@ -515,53 +551,59 @@
       <c r="J18">
         <v>10.050000000000001</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>10.15</v>
-      </c>
-      <c r="N18">
+      <c r="L18">
+        <f t="shared" si="1"/>
         <v>10.050000000000001</v>
       </c>
-      <c r="O18">
-        <f t="shared" si="1"/>
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="19" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="I19" s="1" t="s">
+      <c r="P18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="1">
-        <f t="shared" ref="J19:O19" si="2">SUM(J13:J18)</f>
-        <v>60.149999999999991</v>
-      </c>
-      <c r="K19" s="1">
-        <f t="shared" si="2"/>
-        <v>60.749999999999993</v>
-      </c>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1">
-        <f t="shared" si="2"/>
-        <v>60.149999999999991</v>
-      </c>
-      <c r="O19" s="1">
-        <f t="shared" si="2"/>
-        <v>61.349999999999994</v>
-      </c>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="25" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J25" t="s">
+      <c r="J20">
+        <f>SUM(J13:J18)</f>
+        <v>50.11999999999999</v>
+      </c>
+      <c r="K20">
+        <f>SUM(K13:K18)</f>
+        <v>50.6</v>
+      </c>
+      <c r="L20" s="1">
+        <f>SUM(L13:L18)</f>
+        <v>60.650000000000006</v>
+      </c>
+      <c r="N20">
+        <f>SUM(N13:N18)</f>
+        <v>50.099999999999994</v>
+      </c>
+      <c r="O20">
+        <f>SUM(O13:O18)</f>
+        <v>51.099999999999994</v>
+      </c>
+      <c r="P20" s="1">
+        <f>SUM(P13:P18)</f>
+        <v>51.099999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="J26" t="s">
         <v>5</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>1.19</v>
       </c>
     </row>
-    <row r="27" spans="9:16" x14ac:dyDescent="0.25">
-      <c r="J27" t="s">
+    <row r="28" spans="9:16" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
         <v>6</v>
+      </c>
+      <c r="K28">
+        <f>K26+L20-P20</f>
+        <v>10.740000000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating test case for cash flow calc.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="27795" windowHeight="12840"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20010" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="balance" sheetId="1" r:id="rId1"/>
+    <sheet name="cashflow" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cashflow!$D$6:$G$21</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
+  <pivotCaches>
+    <pivotCache cacheId="7" r:id="rId4"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>actual</t>
   </si>
@@ -41,12 +47,30 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>running sum</t>
+  </si>
+  <si>
+    <t>Sum of running sum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +80,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,14 +111,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -98,6 +138,224 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mario" refreshedDate="41056.767540393521" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="15">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="D6:H21" sheet="cashflow"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="date" numFmtId="16">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2012-03-31T00:00:00" maxDate="2012-04-08T00:00:00" count="8">
+        <d v="2012-03-31T00:00:00"/>
+        <d v="2012-04-01T00:00:00"/>
+        <d v="2012-04-02T00:00:00"/>
+        <d v="2012-04-03T00:00:00"/>
+        <d v="2012-04-04T00:00:00"/>
+        <d v="2012-04-05T00:00:00"/>
+        <d v="2012-04-06T00:00:00"/>
+        <d v="2012-04-07T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="expected" numFmtId="44">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1300" maxValue="1500"/>
+    </cacheField>
+    <cacheField name="actual" numFmtId="44">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1130.21" maxValue="1700.21"/>
+    </cacheField>
+    <cacheField name="considered" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1700.21" maxValue="1500.14"/>
+    </cacheField>
+    <cacheField name="running sum" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-2750.2" maxValue="1430"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="15">
+  <r>
+    <x v="0"/>
+    <n v="1450"/>
+    <n v="1600"/>
+    <n v="-1600"/>
+    <n v="-1600"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1500"/>
+    <n v="1500.1"/>
+    <n v="1500.1"/>
+    <n v="-99.900000000000091"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="1450"/>
+    <n v="1700.21"/>
+    <n v="-1700.21"/>
+    <n v="-1700.21"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="1500"/>
+    <n v="1500.11"/>
+    <n v="1500.11"/>
+    <n v="-200.10000000000014"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="1450"/>
+    <n v="1130.21"/>
+    <n v="-1130.21"/>
+    <n v="-1130.21"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1500"/>
+    <m/>
+    <n v="1500"/>
+    <n v="369.78999999999996"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="1450"/>
+    <n v="1200.21"/>
+    <n v="-1200.21"/>
+    <n v="-1200.21"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <m/>
+    <n v="1500.13"/>
+    <n v="1500.13"/>
+    <n v="299.92000000000007"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="1450"/>
+    <n v="1300.81"/>
+    <n v="-1300.81"/>
+    <n v="-1300.81"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1500"/>
+    <n v="1500.14"/>
+    <n v="1500.14"/>
+    <n v="199.33000000000015"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1500"/>
+    <n v="1430"/>
+    <n v="1430"/>
+    <n v="1430"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1450"/>
+    <n v="1150.22"/>
+    <n v="-1150.22"/>
+    <n v="279.77999999999997"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="1450"/>
+    <n v="1450.2"/>
+    <n v="-1450.2"/>
+    <n v="-1450.2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="1300"/>
+    <m/>
+    <n v="-1300"/>
+    <n v="-2750.2"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="1500"/>
+    <n v="1250"/>
+    <n v="1250"/>
+    <n v="1250"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="K6:L15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" numFmtId="16" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of running sum" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -389,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I11:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +722,7 @@
         <v>10.11</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:L20" si="1">IF(K14 &lt;&gt; "",K14,J14)</f>
+        <f t="shared" ref="L14:L18" si="1">IF(K14 &lt;&gt; "",K14,J14)</f>
         <v>10.11</v>
       </c>
       <c r="N14">
@@ -475,7 +733,7 @@
         <v>10.209999999999999</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:P20" si="3">IF(O14 &lt;&gt; "",O14,N14)</f>
+        <f t="shared" ref="P14:P18" si="3">IF(O14 &lt;&gt; "",O14,N14)</f>
         <v>10.209999999999999</v>
       </c>
     </row>
@@ -614,13 +872,441 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D5:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <v>40999</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1600</v>
+      </c>
+      <c r="G7" s="2">
+        <f>IF(F7 &lt;&gt; "",F7,E7)*-1</f>
+        <v>-1600</v>
+      </c>
+      <c r="H7" s="2">
+        <f>G7</f>
+        <v>-1600</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="K7" s="5">
+        <v>40999</v>
+      </c>
+      <c r="L7" s="6">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <v>41000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1500.1</v>
+      </c>
+      <c r="G8" s="2">
+        <f>IF(F8 &lt;&gt; "",F8,E8)</f>
+        <v>1500.1</v>
+      </c>
+      <c r="H8" s="2">
+        <f>H7+G8</f>
+        <v>-99.900000000000091</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="K8" s="5">
+        <v>41000</v>
+      </c>
+      <c r="L8" s="6">
+        <v>-1800.1100000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <v>41000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1700.21</v>
+      </c>
+      <c r="G9" s="2">
+        <f>IF(F9 &lt;&gt; "",F9,E9)*-1</f>
+        <v>-1700.21</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" ref="H9" si="0">G9</f>
+        <v>-1700.21</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="K9" s="5">
+        <v>41001</v>
+      </c>
+      <c r="L9" s="6">
+        <v>-1330.3100000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <v>41001</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1500.11</v>
+      </c>
+      <c r="G10" s="2">
+        <f>IF(F10 &lt;&gt; "",F10,E10)</f>
+        <v>1500.11</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" ref="H10" si="1">H9+G10</f>
+        <v>-200.10000000000014</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="K10" s="5">
+        <v>41002</v>
+      </c>
+      <c r="L10" s="6">
+        <v>-830.42000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>41001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1130.21</v>
+      </c>
+      <c r="G11" s="2">
+        <f>IF(F11 &lt;&gt; "",F11,E11)*-1</f>
+        <v>-1130.21</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" ref="H11" si="2">G11</f>
+        <v>-1130.21</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="K11" s="5">
+        <v>41003</v>
+      </c>
+      <c r="L11" s="6">
+        <v>-1000.8899999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <v>41002</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <f>IF(F12 &lt;&gt; "",F12,E12)</f>
+        <v>1500</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" ref="H12" si="3">H11+G12</f>
+        <v>369.78999999999996</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="K12" s="5">
+        <v>41004</v>
+      </c>
+      <c r="L12" s="6">
+        <v>458.91000000000008</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <v>41002</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1200.21</v>
+      </c>
+      <c r="G13" s="2">
+        <f>IF(F13 &lt;&gt; "",F13,E13)*-1</f>
+        <v>-1200.21</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" ref="H13" si="4">G13</f>
+        <v>-1200.21</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="K13" s="5">
+        <v>41005</v>
+      </c>
+      <c r="L13" s="6">
+        <v>-2750.2</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <v>41003</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2">
+        <v>1500.13</v>
+      </c>
+      <c r="G14" s="2">
+        <f>IF(F14 &lt;&gt; "",F14,E14)</f>
+        <v>1500.13</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" ref="H14" si="5">H13+G14</f>
+        <v>299.92000000000007</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="K14" s="5">
+        <v>41006</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <v>41003</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1300.81</v>
+      </c>
+      <c r="G15" s="2">
+        <f>IF(F15 &lt;&gt; "",F15,E15)*-1</f>
+        <v>-1300.81</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" ref="H15" si="6">G15</f>
+        <v>-1300.81</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="K15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="6">
+        <v>-7603.02</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1500.14</v>
+      </c>
+      <c r="G16" s="2">
+        <f>IF(F16 &lt;&gt; "",F16,E16)</f>
+        <v>1500.14</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" ref="H16" si="7">H15+G16</f>
+        <v>199.33000000000015</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1430</v>
+      </c>
+      <c r="G17" s="2">
+        <f>IF(F17 &lt;&gt; "",F17,E17)</f>
+        <v>1430</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" ref="H17" si="8">G17</f>
+        <v>1430</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F18" s="2">
+        <v>1150.22</v>
+      </c>
+      <c r="G18" s="2">
+        <f>IF(F18 &lt;&gt; "",F18,E18)*-1</f>
+        <v>-1150.22</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" ref="H18" si="9">H17+G18</f>
+        <v>279.77999999999997</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1450</v>
+      </c>
+      <c r="F19" s="2">
+        <f>E19+0.2</f>
+        <v>1450.2</v>
+      </c>
+      <c r="G19" s="2">
+        <f>IF(F19 &lt;&gt; "",F19,E19)*-1</f>
+        <v>-1450.2</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" ref="H19" si="10">G19</f>
+        <v>-1450.2</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D20" s="3">
+        <v>41005</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1300</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2">
+        <f>IF(F20 &lt;&gt; "",F20,E20)*-1</f>
+        <v>-1300</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" ref="H20" si="11">H19+G20</f>
+        <v>-2750.2</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D21" s="3">
+        <v>41006</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1250</v>
+      </c>
+      <c r="G21" s="2">
+        <f>IF(F21 &lt;&gt; "",F21,E21)</f>
+        <v>1250</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" ref="H21" si="12">G21</f>
+        <v>1250</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="D6:G21">
+    <sortState ref="D7:G21">
+      <sortCondition ref="D6:D21"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Concluded first iteration to calculate cash flow for a given account.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20010" windowHeight="8235" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="balance" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -60,7 +60,7 @@
     <t>running sum</t>
   </si>
   <si>
-    <t>Sum of running sum</t>
+    <t>Min of running sum</t>
   </si>
 </sst>
 </file>
@@ -115,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -125,6 +125,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -141,7 +142,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mario" refreshedDate="41056.767540393521" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="15">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mario" refreshedDate="41057.970641666667" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="15">
   <cacheSource type="worksheet">
     <worksheetSource ref="D6:H21" sheet="cashflow"/>
   </cacheSource>
@@ -159,7 +160,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="expected" numFmtId="44">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1300" maxValue="1500"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1150.22" maxValue="1500"/>
     </cacheField>
     <cacheField name="actual" numFmtId="44">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1130.21" maxValue="1700.21"/>
@@ -168,7 +169,7 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1700.21" maxValue="1500.14"/>
     </cacheField>
     <cacheField name="running sum" numFmtId="44">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-2750.2" maxValue="1430"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1800.1100000000001" maxValue="1999.04"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -200,97 +201,97 @@
     <n v="1450"/>
     <n v="1700.21"/>
     <n v="-1700.21"/>
-    <n v="-1700.21"/>
+    <n v="-1800.1100000000001"/>
   </r>
   <r>
     <x v="2"/>
     <n v="1500"/>
     <n v="1500.11"/>
     <n v="1500.11"/>
-    <n v="-200.10000000000014"/>
+    <n v="-300.00000000000023"/>
   </r>
   <r>
     <x v="2"/>
     <n v="1450"/>
     <n v="1130.21"/>
     <n v="-1130.21"/>
-    <n v="-1130.21"/>
+    <n v="-1430.2100000000003"/>
   </r>
   <r>
     <x v="3"/>
     <n v="1500"/>
     <m/>
     <n v="1500"/>
-    <n v="369.78999999999996"/>
+    <n v="69.789999999999736"/>
   </r>
   <r>
     <x v="3"/>
     <n v="1450"/>
     <n v="1200.21"/>
     <n v="-1200.21"/>
-    <n v="-1200.21"/>
+    <n v="-1130.4200000000003"/>
   </r>
   <r>
     <x v="4"/>
     <m/>
     <n v="1500.13"/>
     <n v="1500.13"/>
-    <n v="299.92000000000007"/>
+    <n v="369.70999999999981"/>
   </r>
   <r>
     <x v="4"/>
     <n v="1450"/>
     <n v="1300.81"/>
     <n v="-1300.81"/>
-    <n v="-1300.81"/>
+    <n v="-931.10000000000014"/>
   </r>
   <r>
     <x v="5"/>
     <n v="1500"/>
     <n v="1500.14"/>
     <n v="1500.14"/>
-    <n v="199.33000000000015"/>
+    <n v="569.04"/>
   </r>
   <r>
     <x v="5"/>
     <n v="1500"/>
     <n v="1430"/>
     <n v="1430"/>
-    <n v="1430"/>
+    <n v="1999.04"/>
   </r>
   <r>
     <x v="5"/>
     <n v="1450"/>
     <n v="1150.22"/>
     <n v="-1150.22"/>
-    <n v="279.77999999999997"/>
+    <n v="848.81999999999994"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="1450"/>
-    <n v="1450.2"/>
-    <n v="-1450.2"/>
-    <n v="-1450.2"/>
+    <m/>
+    <n v="1300"/>
+    <n v="-1300"/>
+    <n v="-451.18000000000006"/>
   </r>
   <r>
     <x v="6"/>
-    <n v="1300"/>
+    <n v="1150.22"/>
     <m/>
-    <n v="-1300"/>
-    <n v="-2750.2"/>
+    <n v="-1150.22"/>
+    <n v="-1601.4"/>
   </r>
   <r>
     <x v="7"/>
     <n v="1500"/>
     <n v="1250"/>
     <n v="1250"/>
-    <n v="1250"/>
+    <n v="-351.40000000000009"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K6:L15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" numFmtId="16" showAll="0">
@@ -347,7 +348,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Sum of running sum" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Min of running sum" fld="4" subtotal="min" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -874,20 +875,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:12" x14ac:dyDescent="0.25">
@@ -928,7 +930,7 @@
       <c r="F7" s="2">
         <v>1600</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="7">
         <f>IF(F7 &lt;&gt; "",F7,E7)*-1</f>
         <v>-1600</v>
       </c>
@@ -954,7 +956,7 @@
       <c r="F8" s="2">
         <v>1500.1</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="7">
         <f>IF(F8 &lt;&gt; "",F8,E8)</f>
         <v>1500.1</v>
       </c>
@@ -980,20 +982,20 @@
       <c r="F9" s="2">
         <v>1700.21</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="7">
         <f>IF(F9 &lt;&gt; "",F9,E9)*-1</f>
         <v>-1700.21</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9" si="0">G9</f>
-        <v>-1700.21</v>
+        <f>H8+G9</f>
+        <v>-1800.1100000000001</v>
       </c>
       <c r="I9" s="2"/>
       <c r="K9" s="5">
         <v>41001</v>
       </c>
       <c r="L9" s="6">
-        <v>-1330.3100000000002</v>
+        <v>-1430.2100000000003</v>
       </c>
     </row>
     <row r="10" spans="4:12" x14ac:dyDescent="0.25">
@@ -1006,20 +1008,20 @@
       <c r="F10" s="2">
         <v>1500.11</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="7">
         <f>IF(F10 &lt;&gt; "",F10,E10)</f>
         <v>1500.11</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" ref="H10" si="1">H9+G10</f>
-        <v>-200.10000000000014</v>
+        <f t="shared" ref="H10:I21" si="0">H9+G10</f>
+        <v>-300.00000000000023</v>
       </c>
       <c r="I10" s="2"/>
       <c r="K10" s="5">
         <v>41002</v>
       </c>
       <c r="L10" s="6">
-        <v>-830.42000000000007</v>
+        <v>-1130.4200000000003</v>
       </c>
     </row>
     <row r="11" spans="4:12" x14ac:dyDescent="0.25">
@@ -1032,20 +1034,20 @@
       <c r="F11" s="2">
         <v>1130.21</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="7">
         <f>IF(F11 &lt;&gt; "",F11,E11)*-1</f>
         <v>-1130.21</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" ref="H11" si="2">G11</f>
-        <v>-1130.21</v>
+        <f t="shared" si="0"/>
+        <v>-1430.2100000000003</v>
       </c>
       <c r="I11" s="2"/>
       <c r="K11" s="5">
         <v>41003</v>
       </c>
       <c r="L11" s="6">
-        <v>-1000.8899999999999</v>
+        <v>-931.10000000000014</v>
       </c>
     </row>
     <row r="12" spans="4:12" x14ac:dyDescent="0.25">
@@ -1056,20 +1058,20 @@
         <v>1500</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2">
+      <c r="G12" s="7">
         <f>IF(F12 &lt;&gt; "",F12,E12)</f>
         <v>1500</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" ref="H12" si="3">H11+G12</f>
-        <v>369.78999999999996</v>
+        <f t="shared" si="0"/>
+        <v>69.789999999999736</v>
       </c>
       <c r="I12" s="2"/>
       <c r="K12" s="5">
         <v>41004</v>
       </c>
       <c r="L12" s="6">
-        <v>458.91000000000008</v>
+        <v>-451.18000000000006</v>
       </c>
     </row>
     <row r="13" spans="4:12" x14ac:dyDescent="0.25">
@@ -1082,20 +1084,20 @@
       <c r="F13" s="2">
         <v>1200.21</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="7">
         <f>IF(F13 &lt;&gt; "",F13,E13)*-1</f>
         <v>-1200.21</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" ref="H13" si="4">G13</f>
-        <v>-1200.21</v>
+        <f t="shared" si="0"/>
+        <v>-1130.4200000000003</v>
       </c>
       <c r="I13" s="2"/>
       <c r="K13" s="5">
         <v>41005</v>
       </c>
       <c r="L13" s="6">
-        <v>-2750.2</v>
+        <v>-1601.4</v>
       </c>
     </row>
     <row r="14" spans="4:12" x14ac:dyDescent="0.25">
@@ -1106,20 +1108,20 @@
       <c r="F14" s="2">
         <v>1500.13</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="7">
         <f>IF(F14 &lt;&gt; "",F14,E14)</f>
         <v>1500.13</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" ref="H14" si="5">H13+G14</f>
-        <v>299.92000000000007</v>
+        <f t="shared" si="0"/>
+        <v>369.70999999999981</v>
       </c>
       <c r="I14" s="2"/>
       <c r="K14" s="5">
         <v>41006</v>
       </c>
       <c r="L14" s="6">
-        <v>1250</v>
+        <v>-351.40000000000009</v>
       </c>
     </row>
     <row r="15" spans="4:12" x14ac:dyDescent="0.25">
@@ -1132,20 +1134,20 @@
       <c r="F15" s="2">
         <v>1300.81</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="7">
         <f>IF(F15 &lt;&gt; "",F15,E15)*-1</f>
         <v>-1300.81</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" ref="H15" si="6">G15</f>
-        <v>-1300.81</v>
+        <f t="shared" si="0"/>
+        <v>-931.10000000000014</v>
       </c>
       <c r="I15" s="2"/>
       <c r="K15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L15" s="6">
-        <v>-7603.02</v>
+        <v>-1800.1100000000001</v>
       </c>
     </row>
     <row r="16" spans="4:12" x14ac:dyDescent="0.25">
@@ -1158,13 +1160,13 @@
       <c r="F16" s="2">
         <v>1500.14</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="7">
         <f>IF(F16 &lt;&gt; "",F16,E16)</f>
         <v>1500.14</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16" si="7">H15+G16</f>
-        <v>199.33000000000015</v>
+        <f t="shared" si="0"/>
+        <v>569.04</v>
       </c>
       <c r="I16" s="2"/>
     </row>
@@ -1178,13 +1180,13 @@
       <c r="F17" s="2">
         <v>1430</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="7">
         <f>IF(F17 &lt;&gt; "",F17,E17)</f>
         <v>1430</v>
       </c>
       <c r="H17" s="2">
-        <f t="shared" ref="H17" si="8">G17</f>
-        <v>1430</v>
+        <f t="shared" si="0"/>
+        <v>1999.04</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -1198,13 +1200,13 @@
       <c r="F18" s="2">
         <v>1150.22</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="7">
         <f>IF(F18 &lt;&gt; "",F18,E18)*-1</f>
         <v>-1150.22</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" ref="H18" si="9">H17+G18</f>
-        <v>279.77999999999997</v>
+        <f t="shared" si="0"/>
+        <v>848.81999999999994</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="3"/>
@@ -1214,20 +1216,17 @@
       <c r="D19" s="3">
         <v>41004</v>
       </c>
-      <c r="E19" s="2">
-        <v>1450</v>
-      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2">
-        <f>E19+0.2</f>
-        <v>1450.2</v>
-      </c>
-      <c r="G19" s="2">
+        <v>1300</v>
+      </c>
+      <c r="G19" s="7">
         <f>IF(F19 &lt;&gt; "",F19,E19)*-1</f>
-        <v>-1450.2</v>
+        <v>-1300</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" ref="H19" si="10">G19</f>
-        <v>-1450.2</v>
+        <f t="shared" si="0"/>
+        <v>-451.18000000000006</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="3"/>
@@ -1238,16 +1237,16 @@
         <v>41005</v>
       </c>
       <c r="E20" s="2">
-        <v>1300</v>
+        <v>1150.22</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2">
+      <c r="G20" s="7">
         <f>IF(F20 &lt;&gt; "",F20,E20)*-1</f>
-        <v>-1300</v>
+        <v>-1150.22</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" ref="H20" si="11">H19+G20</f>
-        <v>-2750.2</v>
+        <f t="shared" si="0"/>
+        <v>-1601.4</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="3"/>
@@ -1263,13 +1262,13 @@
       <c r="F21" s="2">
         <v>1250</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="7">
         <f>IF(F21 &lt;&gt; "",F21,E21)</f>
         <v>1250</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" ref="H21" si="12">G21</f>
-        <v>1250</v>
+        <f t="shared" si="0"/>
+        <v>-351.40000000000009</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="3"/>
@@ -1305,6 +1304,16 @@
       <sortCondition ref="D6:D21"/>
     </sortState>
   </autoFilter>
+  <conditionalFormatting sqref="G6:G21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing boundary cases for cash flow calculations. More tests needed.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="1"/>
@@ -14,15 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cashflow!$D$6:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
-  <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId4"/>
-  </pivotCaches>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>actual</t>
   </si>
@@ -51,16 +48,13 @@
     <t>date</t>
   </si>
   <si>
-    <t>Row Labels</t>
+    <t>day</t>
   </si>
   <si>
-    <t>Grand Total</t>
+    <t>daily total</t>
   </si>
   <si>
-    <t>running sum</t>
-  </si>
-  <si>
-    <t>Min of running sum</t>
+    <t>runnig sum</t>
   </si>
 </sst>
 </file>
@@ -115,17 +109,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -139,224 +129,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mario" refreshedDate="41057.970641666667" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="15">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="D6:H21" sheet="cashflow"/>
-  </cacheSource>
-  <cacheFields count="5">
-    <cacheField name="date" numFmtId="16">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2012-03-31T00:00:00" maxDate="2012-04-08T00:00:00" count="8">
-        <d v="2012-03-31T00:00:00"/>
-        <d v="2012-04-01T00:00:00"/>
-        <d v="2012-04-02T00:00:00"/>
-        <d v="2012-04-03T00:00:00"/>
-        <d v="2012-04-04T00:00:00"/>
-        <d v="2012-04-05T00:00:00"/>
-        <d v="2012-04-06T00:00:00"/>
-        <d v="2012-04-07T00:00:00"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="expected" numFmtId="44">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1150.22" maxValue="1500"/>
-    </cacheField>
-    <cacheField name="actual" numFmtId="44">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1130.21" maxValue="1700.21"/>
-    </cacheField>
-    <cacheField name="considered" numFmtId="44">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1700.21" maxValue="1500.14"/>
-    </cacheField>
-    <cacheField name="running sum" numFmtId="44">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1800.1100000000001" maxValue="1999.04"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="15">
-  <r>
-    <x v="0"/>
-    <n v="1450"/>
-    <n v="1600"/>
-    <n v="-1600"/>
-    <n v="-1600"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="1500"/>
-    <n v="1500.1"/>
-    <n v="1500.1"/>
-    <n v="-99.900000000000091"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="1450"/>
-    <n v="1700.21"/>
-    <n v="-1700.21"/>
-    <n v="-1800.1100000000001"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="1500"/>
-    <n v="1500.11"/>
-    <n v="1500.11"/>
-    <n v="-300.00000000000023"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="1450"/>
-    <n v="1130.21"/>
-    <n v="-1130.21"/>
-    <n v="-1430.2100000000003"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="1500"/>
-    <m/>
-    <n v="1500"/>
-    <n v="69.789999999999736"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="1450"/>
-    <n v="1200.21"/>
-    <n v="-1200.21"/>
-    <n v="-1130.4200000000003"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <m/>
-    <n v="1500.13"/>
-    <n v="1500.13"/>
-    <n v="369.70999999999981"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="1450"/>
-    <n v="1300.81"/>
-    <n v="-1300.81"/>
-    <n v="-931.10000000000014"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="1500"/>
-    <n v="1500.14"/>
-    <n v="1500.14"/>
-    <n v="569.04"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="1500"/>
-    <n v="1430"/>
-    <n v="1430"/>
-    <n v="1999.04"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="1450"/>
-    <n v="1150.22"/>
-    <n v="-1150.22"/>
-    <n v="848.81999999999994"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <m/>
-    <n v="1300"/>
-    <n v="-1300"/>
-    <n v="-451.18000000000006"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="1150.22"/>
-    <m/>
-    <n v="-1150.22"/>
-    <n v="-1601.4"/>
-  </r>
-  <r>
-    <x v="7"/>
-    <n v="1500"/>
-    <n v="1250"/>
-    <n v="1250"/>
-    <n v="-351.40000000000009"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="K6:L15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" numFmtId="16" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="44" showAll="0"/>
-    <pivotField dataField="1" numFmtId="44" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Min of running sum" fld="4" subtotal="min" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,8 +647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +656,7 @@
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
     <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
@@ -892,12 +664,21 @@
     <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>8</v>
       </c>
@@ -910,17 +691,17 @@
       <c r="G6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D7" s="3">
         <v>40999</v>
       </c>
@@ -930,23 +711,24 @@
       <c r="F7" s="2">
         <v>1600</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <f>IF(F7 &lt;&gt; "",F7,E7)*-1</f>
         <v>-1600</v>
       </c>
-      <c r="H7" s="2">
-        <f>G7</f>
+      <c r="H7" s="2"/>
+      <c r="I7" s="5">
+        <v>40999</v>
+      </c>
+      <c r="J7">
+        <f ca="1">SUMIF($D$7:$G$21,I7,$G$7:$G$21)</f>
         <v>-1600</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="K7" s="5">
-        <v>40999</v>
-      </c>
-      <c r="L7" s="6">
+      <c r="K7">
+        <f ca="1">K6+J7</f>
         <v>-1600</v>
       </c>
     </row>
-    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D8" s="3">
         <v>41000</v>
       </c>
@@ -956,23 +738,24 @@
       <c r="F8" s="2">
         <v>1500.1</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4">
         <f>IF(F8 &lt;&gt; "",F8,E8)</f>
         <v>1500.1</v>
       </c>
-      <c r="H8" s="2">
-        <f>H7+G8</f>
-        <v>-99.900000000000091</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="K8" s="5">
+      <c r="H8" s="2"/>
+      <c r="I8" s="5">
         <v>41000</v>
       </c>
-      <c r="L8" s="6">
+      <c r="J8">
+        <f ca="1">SUMIF($D$7:$G$21,I8,$G$7:$G$21)</f>
+        <v>-200.11000000000013</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ref="K8:K21" ca="1" si="0">K7+J8</f>
         <v>-1800.1100000000001</v>
       </c>
     </row>
-    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D9" s="3">
         <v>41000</v>
       </c>
@@ -982,23 +765,24 @@
       <c r="F9" s="2">
         <v>1700.21</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <f>IF(F9 &lt;&gt; "",F9,E9)*-1</f>
         <v>-1700.21</v>
       </c>
-      <c r="H9" s="2">
-        <f>H8+G9</f>
-        <v>-1800.1100000000001</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="K9" s="5">
+      <c r="H9" s="2"/>
+      <c r="I9" s="5">
         <v>41001</v>
       </c>
-      <c r="L9" s="6">
+      <c r="J9">
+        <f ca="1">SUMIF($D$7:$G$21,I9,$G$7:$G$21)</f>
+        <v>369.89999999999986</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="0"/>
         <v>-1430.2100000000003</v>
       </c>
     </row>
-    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D10" s="3">
         <v>41001</v>
       </c>
@@ -1008,23 +792,24 @@
       <c r="F10" s="2">
         <v>1500.11</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <f>IF(F10 &lt;&gt; "",F10,E10)</f>
         <v>1500.11</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" ref="H10:I21" si="0">H9+G10</f>
-        <v>-300.00000000000023</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="K10" s="5">
+      <c r="H10" s="2"/>
+      <c r="I10" s="5">
         <v>41002</v>
       </c>
-      <c r="L10" s="6">
+      <c r="J10">
+        <f ca="1">SUMIF($D$7:$G$21,I10,$G$7:$G$21)</f>
+        <v>299.78999999999996</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="0"/>
         <v>-1130.4200000000003</v>
       </c>
     </row>
-    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D11" s="3">
         <v>41001</v>
       </c>
@@ -1034,23 +819,24 @@
       <c r="F11" s="2">
         <v>1130.21</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <f>IF(F11 &lt;&gt; "",F11,E11)*-1</f>
         <v>-1130.21</v>
       </c>
-      <c r="H11" s="2">
-        <f t="shared" si="0"/>
-        <v>-1430.2100000000003</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="K11" s="5">
+      <c r="H11" s="2"/>
+      <c r="I11" s="5">
         <v>41003</v>
       </c>
-      <c r="L11" s="6">
+      <c r="J11">
+        <f ca="1">SUMIF($D$7:$G$21,I11,$G$7:$G$21)</f>
+        <v>199.32000000000016</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
         <v>-931.10000000000014</v>
       </c>
     </row>
-    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D12" s="3">
         <v>41002</v>
       </c>
@@ -1058,23 +844,24 @@
         <v>1500</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <f>IF(F12 &lt;&gt; "",F12,E12)</f>
         <v>1500</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="0"/>
-        <v>69.789999999999736</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="K12" s="5">
+      <c r="H12" s="2"/>
+      <c r="I12" s="5">
         <v>41004</v>
       </c>
-      <c r="L12" s="6">
-        <v>-451.18000000000006</v>
-      </c>
-    </row>
-    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f ca="1">SUMIF($D$7:$G$21,I12,$G$7:$G$21)</f>
+        <v>479.9200000000003</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
+        <v>-451.17999999999984</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D13" s="3">
         <v>41002</v>
       </c>
@@ -1084,23 +871,24 @@
       <c r="F13" s="2">
         <v>1200.21</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <f>IF(F13 &lt;&gt; "",F13,E13)*-1</f>
         <v>-1200.21</v>
       </c>
-      <c r="H13" s="2">
-        <f t="shared" si="0"/>
-        <v>-1130.4200000000003</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="K13" s="5">
+      <c r="H13" s="2"/>
+      <c r="I13" s="5">
         <v>41005</v>
       </c>
-      <c r="L13" s="6">
-        <v>-1601.4</v>
-      </c>
-    </row>
-    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f ca="1">SUMIF($D$7:$G$21,I13,$G$7:$G$21)</f>
+        <v>-1150.22</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1601.3999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D14" s="3">
         <v>41003</v>
       </c>
@@ -1108,23 +896,24 @@
       <c r="F14" s="2">
         <v>1500.13</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <f>IF(F14 &lt;&gt; "",F14,E14)</f>
         <v>1500.13</v>
       </c>
-      <c r="H14" s="2">
-        <f t="shared" si="0"/>
-        <v>369.70999999999981</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="K14" s="5">
+      <c r="H14" s="2"/>
+      <c r="I14" s="5">
         <v>41006</v>
       </c>
-      <c r="L14" s="6">
-        <v>-351.40000000000009</v>
-      </c>
-    </row>
-    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f ca="1">SUMIF($D$7:$G$21,I14,$G$7:$G$21)</f>
+        <v>1250</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="0"/>
+        <v>-351.39999999999986</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D15" s="3">
         <v>41003</v>
       </c>
@@ -1134,23 +923,24 @@
       <c r="F15" s="2">
         <v>1300.81</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <f>IF(F15 &lt;&gt; "",F15,E15)*-1</f>
         <v>-1300.81</v>
       </c>
-      <c r="H15" s="2">
-        <f t="shared" si="0"/>
-        <v>-931.10000000000014</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="K15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L15" s="6">
-        <v>-1800.1100000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+      <c r="I15" s="5">
+        <v>41007</v>
+      </c>
+      <c r="J15">
+        <f ca="1">SUMIF($D$7:$G$21,I15,$G$7:$G$21)</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="0"/>
+        <v>-351.39999999999986</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D16" s="3">
         <v>41004</v>
       </c>
@@ -1160,15 +950,22 @@
       <c r="F16" s="2">
         <v>1500.14</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <f>IF(F16 &lt;&gt; "",F16,E16)</f>
         <v>1500.14</v>
       </c>
-      <c r="H16" s="2">
-        <f t="shared" si="0"/>
-        <v>569.04</v>
-      </c>
-      <c r="I16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="5">
+        <v>41008</v>
+      </c>
+      <c r="J16">
+        <f ca="1">SUMIF($D$7:$G$21,I16,$G$7:$G$21)</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="0"/>
+        <v>-351.39999999999986</v>
+      </c>
     </row>
     <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" s="3">
@@ -1180,15 +977,12 @@
       <c r="F17" s="2">
         <v>1430</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <f>IF(F17 &lt;&gt; "",F17,E17)</f>
         <v>1430</v>
       </c>
-      <c r="H17" s="2">
-        <f t="shared" si="0"/>
-        <v>1999.04</v>
-      </c>
-      <c r="I17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D18" s="3">
@@ -1200,16 +994,12 @@
       <c r="F18" s="2">
         <v>1150.22</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <f>IF(F18 &lt;&gt; "",F18,E18)*-1</f>
         <v>-1150.22</v>
       </c>
-      <c r="H18" s="2">
-        <f t="shared" si="0"/>
-        <v>848.81999999999994</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
@@ -1220,16 +1010,12 @@
       <c r="F19" s="2">
         <v>1300</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <f>IF(F19 &lt;&gt; "",F19,E19)*-1</f>
         <v>-1300</v>
       </c>
-      <c r="H19" s="2">
-        <f t="shared" si="0"/>
-        <v>-451.18000000000006</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="4:13" x14ac:dyDescent="0.25">
@@ -1240,16 +1026,12 @@
         <v>1150.22</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <f>IF(F20 &lt;&gt; "",F20,E20)*-1</f>
         <v>-1150.22</v>
       </c>
-      <c r="H20" s="2">
-        <f t="shared" si="0"/>
-        <v>-1601.4</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="5"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="4:13" x14ac:dyDescent="0.25">
@@ -1262,17 +1044,12 @@
       <c r="F21" s="2">
         <v>1250</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <f>IF(F21 &lt;&gt; "",F21,E21)</f>
         <v>1250</v>
       </c>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>-351.40000000000009</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="5"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
@@ -1315,7 +1092,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Scenarios for cash flow calc with multiple accounts.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="balance" sheetId="1" r:id="rId1"/>
     <sheet name="cashflow" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="cashflow (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cashflow!$D$6:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'cashflow (2)'!$D$6:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId5"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>actual</t>
   </si>
@@ -56,13 +61,30 @@
   <si>
     <t>runnig sum</t>
   </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Sum of considered</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -105,19 +127,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -129,6 +160,249 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Mario" refreshedDate="41065.933452777776" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="15">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="C6:G21" sheet="cashflow (2)"/>
+  </cacheSource>
+  <cacheFields count="5">
+    <cacheField name="Account" numFmtId="165">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
+        <n v="1"/>
+        <n v="4"/>
+        <n v="3"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="date" numFmtId="16">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2012-03-31T00:00:00" maxDate="2012-04-08T00:00:00" count="8">
+        <d v="2012-04-01T00:00:00"/>
+        <d v="2012-04-05T00:00:00"/>
+        <d v="2012-04-07T00:00:00"/>
+        <d v="2012-04-02T00:00:00"/>
+        <d v="2012-04-03T00:00:00"/>
+        <d v="2012-04-04T00:00:00"/>
+        <d v="2012-03-31T00:00:00"/>
+        <d v="2012-04-06T00:00:00"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="expected" numFmtId="44">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="-1450" maxValue="1500"/>
+    </cacheField>
+    <cacheField name="actual" numFmtId="44">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-1700.21" maxValue="1500.14"/>
+    </cacheField>
+    <cacheField name="considered" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-1700.21" maxValue="1500.14"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="15">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1500"/>
+    <n v="1500.1"/>
+    <n v="1500.1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1500"/>
+    <n v="1500.14"/>
+    <n v="1500.14"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1500"/>
+    <n v="1430"/>
+    <n v="1430"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="1500"/>
+    <n v="1250"/>
+    <n v="1250"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="1500"/>
+    <n v="1500.11"/>
+    <n v="1500.11"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="1500"/>
+    <m/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="1500"/>
+    <n v="1500.13"/>
+    <n v="1500.13"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="-1450"/>
+    <n v="-1600"/>
+    <n v="-1600"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="-1450"/>
+    <n v="-1700.21"/>
+    <n v="-1700.21"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="-1300"/>
+    <m/>
+    <n v="-1300"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="7"/>
+    <m/>
+    <n v="-1150.22"/>
+    <n v="-1150.22"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="-1450"/>
+    <n v="-1130.21"/>
+    <n v="-1130.21"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="-1450"/>
+    <n v="-1200.21"/>
+    <n v="-1200.21"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="-1450"/>
+    <n v="-1300.81"/>
+    <n v="-1300.81"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="-1450"/>
+    <n v="-1150.22"/>
+    <n v="-1150.22"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G29:K39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisCol" numFmtId="165" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" numFmtId="16" showAll="0">
+      <items count="9">
+        <item x="6"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of considered" fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D5:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,7 +994,7 @@
         <v>40999</v>
       </c>
       <c r="J7">
-        <f ca="1">SUMIF($D$7:$G$21,I7,$G$7:$G$21)</f>
+        <f t="shared" ref="J7:J16" ca="1" si="0">SUMIF($D$7:$G$21,I7,$G$7:$G$21)</f>
         <v>-1600</v>
       </c>
       <c r="K7">
@@ -747,11 +1021,11 @@
         <v>41000</v>
       </c>
       <c r="J8">
-        <f ca="1">SUMIF($D$7:$G$21,I8,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-200.11000000000013</v>
       </c>
       <c r="K8">
-        <f t="shared" ref="K8:K21" ca="1" si="0">K7+J8</f>
+        <f t="shared" ref="K8:K16" ca="1" si="1">K7+J8</f>
         <v>-1800.1100000000001</v>
       </c>
     </row>
@@ -774,11 +1048,11 @@
         <v>41001</v>
       </c>
       <c r="J9">
-        <f ca="1">SUMIF($D$7:$G$21,I9,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>369.89999999999986</v>
       </c>
       <c r="K9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-1430.2100000000003</v>
       </c>
     </row>
@@ -801,11 +1075,11 @@
         <v>41002</v>
       </c>
       <c r="J10">
-        <f ca="1">SUMIF($D$7:$G$21,I10,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>299.78999999999996</v>
       </c>
       <c r="K10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-1130.4200000000003</v>
       </c>
     </row>
@@ -828,11 +1102,11 @@
         <v>41003</v>
       </c>
       <c r="J11">
-        <f ca="1">SUMIF($D$7:$G$21,I11,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>199.32000000000016</v>
       </c>
       <c r="K11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-931.10000000000014</v>
       </c>
     </row>
@@ -853,11 +1127,11 @@
         <v>41004</v>
       </c>
       <c r="J12">
-        <f ca="1">SUMIF($D$7:$G$21,I12,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>479.9200000000003</v>
       </c>
       <c r="K12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-451.17999999999984</v>
       </c>
     </row>
@@ -880,11 +1154,11 @@
         <v>41005</v>
       </c>
       <c r="J13">
-        <f ca="1">SUMIF($D$7:$G$21,I13,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>-1150.22</v>
       </c>
       <c r="K13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-1601.3999999999999</v>
       </c>
     </row>
@@ -905,11 +1179,11 @@
         <v>41006</v>
       </c>
       <c r="J14">
-        <f ca="1">SUMIF($D$7:$G$21,I14,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1250</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-351.39999999999986</v>
       </c>
     </row>
@@ -932,11 +1206,11 @@
         <v>41007</v>
       </c>
       <c r="J15">
-        <f ca="1">SUMIF($D$7:$G$21,I15,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="K15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-351.39999999999986</v>
       </c>
     </row>
@@ -959,11 +1233,11 @@
         <v>41008</v>
       </c>
       <c r="J16">
-        <f ca="1">SUMIF($D$7:$G$21,I16,$G$7:$G$21)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>-351.39999999999986</v>
       </c>
     </row>
@@ -1098,6 +1372,546 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:M39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32:H34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="21" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>41000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1500.1</v>
+      </c>
+      <c r="G7" s="4">
+        <f>IF(F7 &lt;&gt; "",F7,E7)</f>
+        <v>1500.1</v>
+      </c>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1500.14</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:G21" si="0">IF(F8 &lt;&gt; "",F8,E8)</f>
+        <v>1500.14</v>
+      </c>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="6">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1430</v>
+      </c>
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>1430</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>41006</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1250</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>1250</v>
+      </c>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="6">
+        <v>4</v>
+      </c>
+      <c r="D11" s="3">
+        <v>41001</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1500.11</v>
+      </c>
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>1500.11</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="6">
+        <v>3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>41002</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>41003</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1500</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1500.13</v>
+      </c>
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>1500.13</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="6">
+        <v>3</v>
+      </c>
+      <c r="D14" s="3">
+        <v>40999</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F14" s="2">
+        <v>-1600</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
+        <v>-1600</v>
+      </c>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3">
+        <v>41000</v>
+      </c>
+      <c r="E15" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F15" s="2">
+        <v>-1700.21</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>-1700.21</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-1300</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>-1300</v>
+      </c>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>41005</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
+        <v>-1150.22</v>
+      </c>
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>-1150.22</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3">
+        <v>41001</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F18" s="2">
+        <v>-1130.21</v>
+      </c>
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>-1130.21</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="5"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C19" s="6">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>41002</v>
+      </c>
+      <c r="E19" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F19" s="2">
+        <v>-1200.21</v>
+      </c>
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>-1200.21</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="5"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C20" s="6">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3">
+        <v>41003</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-1300.81</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>-1300.81</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="5"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C21" s="6">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>41004</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-1450</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-1150.22</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>-1150.22</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="5"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>3</v>
+      </c>
+      <c r="J30" s="10">
+        <v>4</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G31" s="8">
+        <v>40999</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9">
+        <v>-1600</v>
+      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="G32" s="8">
+        <v>41000</v>
+      </c>
+      <c r="H32" s="9">
+        <v>-200.11000000000013</v>
+      </c>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9">
+        <v>-200.11000000000013</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G33" s="8">
+        <v>41001</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9">
+        <v>369.89999999999986</v>
+      </c>
+      <c r="K33" s="9">
+        <v>369.89999999999986</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="8">
+        <v>41002</v>
+      </c>
+      <c r="H34" s="9">
+        <v>-1200.21</v>
+      </c>
+      <c r="I34" s="9">
+        <v>1500</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9">
+        <v>299.78999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <v>41003</v>
+      </c>
+      <c r="H35" s="9">
+        <v>1500.13</v>
+      </c>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9">
+        <v>-1300.81</v>
+      </c>
+      <c r="K35" s="9">
+        <v>199.32000000000016</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G36" s="8">
+        <v>41004</v>
+      </c>
+      <c r="H36" s="9">
+        <v>349.92000000000007</v>
+      </c>
+      <c r="I36" s="9">
+        <v>-1300</v>
+      </c>
+      <c r="J36" s="9">
+        <v>1430</v>
+      </c>
+      <c r="K36" s="9">
+        <v>479.92000000000007</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G37" s="8">
+        <v>41005</v>
+      </c>
+      <c r="H37" s="9">
+        <v>-1150.22</v>
+      </c>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9">
+        <v>-1150.22</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G38" s="8">
+        <v>41006</v>
+      </c>
+      <c r="H38" s="9">
+        <v>1250</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G39" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H39" s="9">
+        <v>549.51</v>
+      </c>
+      <c r="I39" s="9">
+        <v>-1400</v>
+      </c>
+      <c r="J39" s="9">
+        <v>499.08999999999992</v>
+      </c>
+      <c r="K39" s="9">
+        <v>-351.40000000000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="D6:G21">
+    <sortState ref="D7:G21">
+      <sortCondition ref="D6:D21"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:G21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <color rgb="FFFF7128"/>
+        <color rgb="FFFFEF9C"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Started summary calculations for the first tab of the side panel.
</commit_message>
<xml_diff>
--- a/docs/scenarios.xlsx
+++ b/docs/scenarios.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20010" windowHeight="8175" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="balance" sheetId="1" r:id="rId1"/>
     <sheet name="cashflow" sheetId="2" r:id="rId2"/>
     <sheet name="cashflow (2)" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="summary calcs" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cashflow!$D$6:$G$21</definedName>
@@ -18,13 +18,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>actual</t>
   </si>
@@ -76,6 +76,9 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>dia</t>
+  </si>
 </sst>
 </file>
 
@@ -84,7 +87,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -139,13 +142,13 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -168,7 +171,7 @@
     <worksheetSource ref="C6:G21" sheet="cashflow (2)"/>
   </cacheSource>
   <cacheFields count="5">
-    <cacheField name="Account" numFmtId="165">
+    <cacheField name="Account" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4" count="3">
         <n v="1"/>
         <n v="4"/>
@@ -316,10 +319,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G29:K39" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
-    <pivotField axis="axisCol" numFmtId="165" showAll="0">
+    <pivotField axis="axisCol" numFmtId="164" showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="2"/>
@@ -1374,7 +1377,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C6:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H32" sqref="H32:H34"/>
     </sheetView>
   </sheetViews>
@@ -1912,12 +1915,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="D7:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>10.01</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>10.02</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>10.029999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>10.039999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>